<commit_message>
Add BOM spreadsheet and related images
Added BOM.xlsx and two images (BOM.png and Schéma.png) to provide documentation and visual references for the bill of materials and schematic.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\OneDrive\Documents\GitHub\My-Home-Assisant-Box\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6792CD1D-216A-4D32-98F1-1403A0BB08DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CBEF9A-B3D3-4BF9-9DC3-C6A9855A499D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-119" yWindow="-119" windowWidth="28741" windowHeight="16271" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,13 +446,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.8" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" customWidth="1"/>
     <col min="5" max="5" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -492,7 +492,7 @@
         <v>65.7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -512,7 +512,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -532,7 +532,7 @@
         <v>20.39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -552,7 +552,7 @@
         <v>13.99</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -572,7 +572,7 @@
         <v>2.5099999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -592,7 +592,7 @@
         <v>6.09</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -612,7 +612,7 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -632,7 +632,7 @@
         <v>1.59</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -652,7 +652,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -672,7 +672,7 @@
         <v>4.59</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -692,7 +692,7 @@
         <v>2.19</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -712,7 +712,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Add 3D models and migrate KiCad schematics
Added STEP files for BackPlate, Box, and Top, and moved corresponding STL files to a new directory. Migrated KiCad schematic and PCB files to a new folder structure. Updated BOM files to reflect these changes.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\OneDrive\Documents\GitHub\My-Home-Assisant-Box\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CBEF9A-B3D3-4BF9-9DC3-C6A9855A499D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18354B1-4568-4B91-894D-2C7DE18320BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-119" yWindow="-119" windowWidth="28741" windowHeight="16271" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>Item Count</t>
   </si>
@@ -43,12 +43,6 @@
     <t>Raspberry Pi 4 Model B</t>
   </si>
   <si>
-    <t>Main Server (4GB RAM)</t>
-  </si>
-  <si>
-    <t>Raspberry Pi 4B - 4GB</t>
-  </si>
-  <si>
     <t>USB-C Power Supply</t>
   </si>
   <si>
@@ -70,12 +64,6 @@
     <t>Micro SD Card</t>
   </si>
   <si>
-    <t>32GB or 64GB Class 10</t>
-  </si>
-  <si>
-    <t>SanDisk 64 Go Extreme microSDXC</t>
-  </si>
-  <si>
     <t>D1 Mini ESP8266</t>
   </si>
   <si>
@@ -148,13 +136,16 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>Potentiometer</t>
-  </si>
-  <si>
-    <t>100Ohm (Fan Speed Control)</t>
-  </si>
-  <si>
-    <t>Potentiometer 200 Ohms</t>
+    <t>PNY 16 Go Extreme microSDXC</t>
+  </si>
+  <si>
+    <t>16GB Class 10</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 4B - 2GB</t>
+  </si>
+  <si>
+    <t>Main Server (2GB RAM)</t>
   </si>
 </sst>
 </file>
@@ -438,21 +429,21 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.8" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
     <col min="5" max="5" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -480,265 +471,245 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
+      <c r="E2" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="F2" s="3">
-        <v>65.7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="F3" s="3">
         <v>6.9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="F4" s="3">
         <v>20.39</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
+      <c r="E5" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="F5" s="3">
-        <v>13.99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
+        <v>11.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F6" s="3">
-        <v>2.5099999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F7" s="3">
-        <v>6.09</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F8" s="3">
         <v>15.9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F9" s="3">
         <v>1.59</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F10" s="3">
         <v>3.79</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F11" s="3">
         <v>4.59</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F12" s="3">
         <v>2.19</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="12.65" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="F14" s="3">
-        <v>1.34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="3">
-        <f>SUM(F2:F14)</f>
-        <v>144.98000000000002</v>
+        <f>SUM(F2:F13)</f>
+        <v>125.68000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -754,10 +725,9 @@
     <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="E12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E14" r:id="rId12" xr:uid="{6553C506-35C3-424E-B7EC-E3801913A13C}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd" r:id="rId13"/>
+  <pageSetup paperSize="9" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>